<commit_message>
modified test case file with Test Case IDs
</commit_message>
<xml_diff>
--- a/TestCaseFile/TestCases_Selenium_GUI.xlsx
+++ b/TestCaseFile/TestCases_Selenium_GUI.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MiniProject\Team_One_Opencart\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MiniProject\Team_One_Opencart\TestCaseFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B664943F-EFF4-4DCB-A594-40CDDB0FB37C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49576BD6-D31B-466C-81EE-374AD3AE6779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>Project Name:</t>
   </si>
@@ -82,23 +82,6 @@
   </si>
   <si>
     <t>Actual Result</t>
-  </si>
-  <si>
-    <t>AUT URL: http://localhost/ecommerce/index.php
-Email: test123@gmail.com
-Password: 12345</t>
-  </si>
-  <si>
-    <t>1. Enter Email in Email field.
-2. Password Email in Password field.
-3. Press "Log In" button to login.
-4.Order Product</t>
-  </si>
-  <si>
-    <t>1. Email is displayed in email field.
-2. Dots representing password characters are displayed in password field.
-3. Log In Button is clickable and loads user login.
-4.Product ordered successfully.</t>
   </si>
   <si>
     <t>OpenCart (Locally Hosted)</t>
@@ -112,6 +95,81 @@
   </si>
   <si>
     <t>13th Nov 2021</t>
+  </si>
+  <si>
+    <t>YS_01</t>
+  </si>
+  <si>
+    <t>SJ_01</t>
+  </si>
+  <si>
+    <t>AS_01</t>
+  </si>
+  <si>
+    <t>AJ_01</t>
+  </si>
+  <si>
+    <t>VT_01</t>
+  </si>
+  <si>
+    <t>YS_02</t>
+  </si>
+  <si>
+    <t>YS_03</t>
+  </si>
+  <si>
+    <t>YS_04</t>
+  </si>
+  <si>
+    <t>YS_05</t>
+  </si>
+  <si>
+    <t>SJ_02</t>
+  </si>
+  <si>
+    <t>SJ_03</t>
+  </si>
+  <si>
+    <t>SJ_04</t>
+  </si>
+  <si>
+    <t>SJ_05</t>
+  </si>
+  <si>
+    <t>AS_02</t>
+  </si>
+  <si>
+    <t>AS_03</t>
+  </si>
+  <si>
+    <t>AS_04</t>
+  </si>
+  <si>
+    <t>AS_05</t>
+  </si>
+  <si>
+    <t>AJ_05</t>
+  </si>
+  <si>
+    <t>AJ_02</t>
+  </si>
+  <si>
+    <t>AJ_03</t>
+  </si>
+  <si>
+    <t>AJ_04</t>
+  </si>
+  <si>
+    <t>VT_02</t>
+  </si>
+  <si>
+    <t>VT_03</t>
+  </si>
+  <si>
+    <t>VT_04</t>
+  </si>
+  <si>
+    <t>VT_05</t>
   </si>
 </sst>
 </file>
@@ -430,15 +488,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -516,12 +565,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -561,6 +604,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -844,7 +902,7 @@
   <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -862,14 +920,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="43" t="s">
-        <v>23</v>
+      <c r="A1" s="54" t="s">
+        <v>20</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
@@ -878,17 +936,17 @@
         <v>4</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I1" s="7"/>
       <c r="J1" s="8"/>
     </row>
     <row r="2" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="44"/>
+      <c r="A2" s="55"/>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="39" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="3"/>
@@ -898,17 +956,17 @@
         <v>5</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I2" s="7"/>
       <c r="J2" s="8"/>
     </row>
     <row r="3" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="45"/>
+      <c r="A3" s="40"/>
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="39" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="10"/>
@@ -918,13 +976,13 @@
         <v>6</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I3" s="7"/>
       <c r="J3" s="8"/>
     </row>
     <row r="4" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="46"/>
+      <c r="A4" s="41"/>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -938,7 +996,7 @@
       <c r="J4" s="8"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="47"/>
+      <c r="A5" s="42"/>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
@@ -950,486 +1008,530 @@
       <c r="J5" s="8"/>
     </row>
     <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.35">
-      <c r="A6" s="48"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="58"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="17"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
+      <c r="A7" s="14"/>
+      <c r="B7" s="56"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="57"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="57"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="17"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
+      <c r="A8" s="14"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="19"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="49" t="s">
+      <c r="A10" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="22" t="s">
+      <c r="F10" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="22" t="s">
+      <c r="G10" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="22" t="s">
+      <c r="H10" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="22" t="s">
+      <c r="I10" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="J10" s="22" t="s">
+      <c r="J10" s="19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="67.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="23"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="H11" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="I11" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="J11" s="23"/>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="20"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="23"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="41"/>
-      <c r="J12" s="23"/>
+      <c r="A12" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="20"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="23"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="23"/>
+      <c r="A13" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="20"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="23"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="23"/>
+      <c r="A14" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="20"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="23"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="23"/>
+      <c r="A15" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="20"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="31"/>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="31"/>
+      <c r="A16" s="28"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="28"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A17" s="23"/>
-      <c r="B17" s="34"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="23"/>
+      <c r="A17" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="31"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="20"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A18" s="23"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="27"/>
-      <c r="I18" s="27"/>
-      <c r="J18" s="23"/>
+      <c r="A18" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="31"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="20"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A19" s="23"/>
-      <c r="B19" s="34"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="23"/>
+      <c r="A19" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="31"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="20"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A20" s="23"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="23"/>
+      <c r="A20" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="20"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A21" s="23"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="23"/>
+      <c r="A21" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="20"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A22" s="31"/>
-      <c r="B22" s="32"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="31"/>
-      <c r="I22" s="31"/>
-      <c r="J22" s="31"/>
+      <c r="A22" s="28"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="28"/>
+      <c r="J22" s="28"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A23" s="23"/>
-      <c r="B23" s="24"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="23"/>
+      <c r="A23" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="20"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A24" s="37"/>
-      <c r="B24" s="24"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="23"/>
+      <c r="A24" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A25" s="23"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="23"/>
+      <c r="A25" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="23"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="20"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A26" s="23"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="26"/>
-      <c r="J26" s="23"/>
+      <c r="A26" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="23"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="20"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A27" s="23"/>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="39"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="26"/>
-      <c r="J27" s="23"/>
+      <c r="A27" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="20"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A28" s="31"/>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
-      <c r="I28" s="31"/>
-      <c r="J28" s="31"/>
+      <c r="A28" s="28"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="28"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A29" s="23"/>
-      <c r="B29" s="24"/>
-      <c r="C29" s="24"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="23"/>
+      <c r="A29" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="20"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A30" s="23"/>
-      <c r="B30" s="34"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="23"/>
+      <c r="A30" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="31"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A31" s="23"/>
-      <c r="B31" s="24"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="28"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="23"/>
-      <c r="H31" s="26"/>
-      <c r="I31" s="26"/>
-      <c r="J31" s="23"/>
+      <c r="A31" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="23"/>
+      <c r="I31" s="23"/>
+      <c r="J31" s="20"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A32" s="23"/>
-      <c r="B32" s="24"/>
-      <c r="C32" s="24"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="28"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="40"/>
-      <c r="H32" s="26"/>
-      <c r="I32" s="26"/>
-      <c r="J32" s="23"/>
+      <c r="A32" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" s="21"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="23"/>
+      <c r="J32" s="20"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A33" s="50"/>
-      <c r="B33" s="51"/>
-      <c r="C33" s="51"/>
-      <c r="D33" s="51"/>
-      <c r="E33" s="52"/>
-      <c r="F33" s="50"/>
-      <c r="G33" s="50"/>
-      <c r="H33" s="53"/>
-      <c r="I33" s="50"/>
-      <c r="J33" s="50"/>
+      <c r="A33" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33" s="46"/>
+      <c r="C33" s="46"/>
+      <c r="D33" s="46"/>
+      <c r="E33" s="47"/>
+      <c r="F33" s="45"/>
+      <c r="G33" s="45"/>
+      <c r="H33" s="48"/>
+      <c r="I33" s="45"/>
+      <c r="J33" s="45"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A34" s="56"/>
-      <c r="B34" s="57"/>
-      <c r="C34" s="58"/>
-      <c r="D34" s="58"/>
-      <c r="E34" s="58"/>
-      <c r="F34" s="58"/>
-      <c r="G34" s="58"/>
-      <c r="H34" s="58"/>
-      <c r="I34" s="58"/>
-      <c r="J34" s="58"/>
+      <c r="A34" s="51"/>
+      <c r="B34" s="52"/>
+      <c r="C34" s="53"/>
+      <c r="D34" s="53"/>
+      <c r="E34" s="53"/>
+      <c r="F34" s="53"/>
+      <c r="G34" s="53"/>
+      <c r="H34" s="53"/>
+      <c r="I34" s="53"/>
+      <c r="J34" s="53"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A35" s="47"/>
-      <c r="B35" s="54"/>
-      <c r="C35" s="55"/>
-      <c r="D35" s="55"/>
-      <c r="E35" s="55"/>
-      <c r="F35" s="55"/>
-      <c r="G35" s="55"/>
-      <c r="H35" s="55"/>
-      <c r="I35" s="55"/>
-      <c r="J35" s="55"/>
+      <c r="A35" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="B35" s="49"/>
+      <c r="C35" s="50"/>
+      <c r="D35" s="50"/>
+      <c r="E35" s="50"/>
+      <c r="F35" s="50"/>
+      <c r="G35" s="50"/>
+      <c r="H35" s="50"/>
+      <c r="I35" s="50"/>
+      <c r="J35" s="50"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A36" s="47"/>
-      <c r="B36" s="54"/>
-      <c r="C36" s="55"/>
-      <c r="D36" s="55"/>
-      <c r="E36" s="55"/>
-      <c r="F36" s="55"/>
-      <c r="G36" s="55"/>
-      <c r="H36" s="55"/>
-      <c r="I36" s="55"/>
-      <c r="J36" s="55"/>
+      <c r="A36" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36" s="49"/>
+      <c r="C36" s="50"/>
+      <c r="D36" s="50"/>
+      <c r="E36" s="50"/>
+      <c r="F36" s="50"/>
+      <c r="G36" s="50"/>
+      <c r="H36" s="50"/>
+      <c r="I36" s="50"/>
+      <c r="J36" s="50"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A37" s="47"/>
-      <c r="B37" s="54"/>
-      <c r="C37" s="55"/>
-      <c r="D37" s="55"/>
-      <c r="E37" s="55"/>
-      <c r="F37" s="55"/>
-      <c r="G37" s="55"/>
-      <c r="H37" s="55"/>
-      <c r="I37" s="55"/>
-      <c r="J37" s="55"/>
+      <c r="A37" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37" s="49"/>
+      <c r="C37" s="50"/>
+      <c r="D37" s="50"/>
+      <c r="E37" s="50"/>
+      <c r="F37" s="50"/>
+      <c r="G37" s="50"/>
+      <c r="H37" s="50"/>
+      <c r="I37" s="50"/>
+      <c r="J37" s="50"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A38" s="47"/>
-      <c r="B38" s="54"/>
-      <c r="C38" s="55"/>
-      <c r="D38" s="55"/>
-      <c r="E38" s="55"/>
-      <c r="F38" s="55"/>
-      <c r="G38" s="55"/>
-      <c r="H38" s="55"/>
-      <c r="I38" s="55"/>
-      <c r="J38" s="55"/>
+      <c r="A38" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38" s="49"/>
+      <c r="C38" s="50"/>
+      <c r="D38" s="50"/>
+      <c r="E38" s="50"/>
+      <c r="F38" s="50"/>
+      <c r="G38" s="50"/>
+      <c r="H38" s="50"/>
+      <c r="I38" s="50"/>
+      <c r="J38" s="50"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A39" s="47"/>
-      <c r="B39" s="54"/>
-      <c r="C39" s="55"/>
-      <c r="D39" s="55"/>
-      <c r="E39" s="55"/>
-      <c r="F39" s="55"/>
-      <c r="G39" s="55"/>
-      <c r="H39" s="55"/>
-      <c r="I39" s="55"/>
-      <c r="J39" s="55"/>
+      <c r="A39" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="B39" s="49"/>
+      <c r="C39" s="50"/>
+      <c r="D39" s="50"/>
+      <c r="E39" s="50"/>
+      <c r="F39" s="50"/>
+      <c r="G39" s="50"/>
+      <c r="H39" s="50"/>
+      <c r="I39" s="50"/>
+      <c r="J39" s="50"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A40" s="47"/>
-      <c r="B40" s="54"/>
-      <c r="C40" s="55"/>
-      <c r="D40" s="55"/>
-      <c r="E40" s="55"/>
-      <c r="F40" s="55"/>
-      <c r="G40" s="55"/>
-      <c r="H40" s="55"/>
-      <c r="I40" s="55"/>
-      <c r="J40" s="55"/>
+      <c r="A40" s="42"/>
+      <c r="B40" s="49"/>
+      <c r="C40" s="50"/>
+      <c r="D40" s="50"/>
+      <c r="E40" s="50"/>
+      <c r="F40" s="50"/>
+      <c r="G40" s="50"/>
+      <c r="H40" s="50"/>
+      <c r="I40" s="50"/>
+      <c r="J40" s="50"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A41" s="47"/>
-      <c r="B41" s="54"/>
-      <c r="C41" s="55"/>
-      <c r="D41" s="55"/>
-      <c r="E41" s="55"/>
-      <c r="F41" s="55"/>
-      <c r="G41" s="55"/>
-      <c r="H41" s="55"/>
-      <c r="I41" s="55"/>
-      <c r="J41" s="55"/>
+      <c r="A41" s="42"/>
+      <c r="B41" s="49"/>
+      <c r="C41" s="50"/>
+      <c r="D41" s="50"/>
+      <c r="E41" s="50"/>
+      <c r="F41" s="50"/>
+      <c r="G41" s="50"/>
+      <c r="H41" s="50"/>
+      <c r="I41" s="50"/>
+      <c r="J41" s="50"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A42" s="47"/>
-      <c r="B42" s="54"/>
-      <c r="C42" s="55"/>
-      <c r="D42" s="55"/>
-      <c r="E42" s="55"/>
-      <c r="F42" s="55"/>
-      <c r="G42" s="55"/>
-      <c r="H42" s="55"/>
-      <c r="I42" s="55"/>
-      <c r="J42" s="55"/>
+      <c r="A42" s="42"/>
+      <c r="B42" s="49"/>
+      <c r="C42" s="50"/>
+      <c r="D42" s="50"/>
+      <c r="E42" s="50"/>
+      <c r="F42" s="50"/>
+      <c r="G42" s="50"/>
+      <c r="H42" s="50"/>
+      <c r="I42" s="50"/>
+      <c r="J42" s="50"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A43" s="55"/>
-      <c r="B43" s="54"/>
-      <c r="C43" s="55"/>
-      <c r="D43" s="55"/>
-      <c r="E43" s="55"/>
-      <c r="F43" s="55"/>
-      <c r="G43" s="55"/>
-      <c r="H43" s="55"/>
-      <c r="I43" s="55"/>
-      <c r="J43" s="55"/>
+      <c r="A43" s="50"/>
+      <c r="B43" s="49"/>
+      <c r="C43" s="50"/>
+      <c r="D43" s="50"/>
+      <c r="E43" s="50"/>
+      <c r="F43" s="50"/>
+      <c r="G43" s="50"/>
+      <c r="H43" s="50"/>
+      <c r="I43" s="50"/>
+      <c r="J43" s="50"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B44" s="1"/>

</xml_diff>

<commit_message>
modified Test Case File with Test_Case_ID
</commit_message>
<xml_diff>
--- a/TestCaseFile/TestCases_Selenium_GUI.xlsx
+++ b/TestCaseFile/TestCases_Selenium_GUI.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MiniProject\Team_One_Opencart\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Persistent_Mini_Project\Team_One_Opencart\TestCaseFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B664943F-EFF4-4DCB-A594-40CDDB0FB37C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA3C8524-7CD4-44AC-ACE0-A152657D9DAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
   <si>
     <t>Project Name:</t>
   </si>
@@ -112,6 +112,69 @@
   </si>
   <si>
     <t>13th Nov 2021</t>
+  </si>
+  <si>
+    <t>YS_01</t>
+  </si>
+  <si>
+    <t>SJ_01</t>
+  </si>
+  <si>
+    <t>AS_01</t>
+  </si>
+  <si>
+    <t>AJ_01</t>
+  </si>
+  <si>
+    <t>VT_01</t>
+  </si>
+  <si>
+    <t>YS_02</t>
+  </si>
+  <si>
+    <t>YS_03</t>
+  </si>
+  <si>
+    <t>YS_04</t>
+  </si>
+  <si>
+    <t>YS_05</t>
+  </si>
+  <si>
+    <t>SJ_02</t>
+  </si>
+  <si>
+    <t>SJ_03</t>
+  </si>
+  <si>
+    <t>SJ_04</t>
+  </si>
+  <si>
+    <t>SJ_05</t>
+  </si>
+  <si>
+    <t>AS_02</t>
+  </si>
+  <si>
+    <t>AS_04</t>
+  </si>
+  <si>
+    <t>AS_03</t>
+  </si>
+  <si>
+    <t>AS_05</t>
+  </si>
+  <si>
+    <t>VT_02</t>
+  </si>
+  <si>
+    <t>VT_03</t>
+  </si>
+  <si>
+    <t>VT_04</t>
+  </si>
+  <si>
+    <t>VT_05</t>
   </si>
 </sst>
 </file>
@@ -430,15 +493,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -516,12 +570,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -561,6 +609,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -843,8 +906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -862,7 +925,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="54" t="s">
         <v>23</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -884,11 +947,11 @@
       <c r="J1" s="8"/>
     </row>
     <row r="2" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="44"/>
+      <c r="A2" s="55"/>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="39" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="3"/>
@@ -904,11 +967,11 @@
       <c r="J2" s="8"/>
     </row>
     <row r="3" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="45"/>
+      <c r="A3" s="40"/>
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="39" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="10"/>
@@ -924,7 +987,7 @@
       <c r="J3" s="8"/>
     </row>
     <row r="4" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="46"/>
+      <c r="A4" s="41"/>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -938,7 +1001,7 @@
       <c r="J4" s="8"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="47"/>
+      <c r="A5" s="42"/>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
@@ -950,486 +1013,536 @@
       <c r="J5" s="8"/>
     </row>
     <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.35">
-      <c r="A6" s="48"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="58"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="17"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
+      <c r="A7" s="14"/>
+      <c r="B7" s="56"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="57"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="57"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="17"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
+      <c r="A8" s="14"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="19"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="49" t="s">
+      <c r="A10" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="22" t="s">
+      <c r="F10" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="22" t="s">
+      <c r="G10" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="22" t="s">
+      <c r="H10" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="22" t="s">
+      <c r="I10" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="J10" s="22" t="s">
+      <c r="J10" s="19" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="67.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="23"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="26" t="s">
+      <c r="A11" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="H11" s="26" t="s">
+      <c r="H11" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="I11" s="26" t="s">
+      <c r="I11" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="J11" s="23"/>
+      <c r="J11" s="20"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="23"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="41"/>
-      <c r="J12" s="23"/>
+      <c r="A12" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="20"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="23"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="23"/>
+      <c r="A13" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="20"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="23"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="23"/>
+      <c r="A14" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="20"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="23"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="23"/>
+      <c r="A15" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="20"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="31"/>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="31"/>
+      <c r="A16" s="28"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="28"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A17" s="23"/>
-      <c r="B17" s="34"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="23"/>
+      <c r="A17" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="31"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="20"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A18" s="23"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="27"/>
-      <c r="I18" s="27"/>
-      <c r="J18" s="23"/>
+      <c r="A18" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="31"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="20"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A19" s="23"/>
-      <c r="B19" s="34"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="23"/>
+      <c r="A19" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="31"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="20"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A20" s="23"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="23"/>
+      <c r="A20" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="20"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A21" s="23"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="23"/>
+      <c r="A21" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="20"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A22" s="31"/>
-      <c r="B22" s="32"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="31"/>
-      <c r="I22" s="31"/>
-      <c r="J22" s="31"/>
+      <c r="A22" s="28"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="28"/>
+      <c r="J22" s="28"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A23" s="23"/>
-      <c r="B23" s="24"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="23"/>
+      <c r="A23" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="20"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A24" s="37"/>
-      <c r="B24" s="24"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="23"/>
+      <c r="A24" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A25" s="23"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="23"/>
+      <c r="A25" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="23"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="20"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A26" s="23"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="26"/>
-      <c r="J26" s="23"/>
+      <c r="A26" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="23"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="20"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A27" s="23"/>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="39"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="26"/>
-      <c r="J27" s="23"/>
+      <c r="A27" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="20"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A28" s="31"/>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
-      <c r="I28" s="31"/>
-      <c r="J28" s="31"/>
+      <c r="A28" s="28"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="28"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A29" s="23"/>
-      <c r="B29" s="24"/>
-      <c r="C29" s="24"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="23"/>
+      <c r="A29" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="20"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A30" s="23"/>
-      <c r="B30" s="34"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="23"/>
+      <c r="A30" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="31"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A31" s="23"/>
-      <c r="B31" s="24"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="28"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="23"/>
-      <c r="H31" s="26"/>
-      <c r="I31" s="26"/>
-      <c r="J31" s="23"/>
+      <c r="A31" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="23"/>
+      <c r="I31" s="23"/>
+      <c r="J31" s="20"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A32" s="23"/>
-      <c r="B32" s="24"/>
-      <c r="C32" s="24"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="28"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="40"/>
-      <c r="H32" s="26"/>
-      <c r="I32" s="26"/>
-      <c r="J32" s="23"/>
+      <c r="A32" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="21"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="23"/>
+      <c r="J32" s="20"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A33" s="50"/>
-      <c r="B33" s="51"/>
-      <c r="C33" s="51"/>
-      <c r="D33" s="51"/>
-      <c r="E33" s="52"/>
-      <c r="F33" s="50"/>
-      <c r="G33" s="50"/>
-      <c r="H33" s="53"/>
-      <c r="I33" s="50"/>
-      <c r="J33" s="50"/>
+      <c r="A33" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" s="46"/>
+      <c r="C33" s="46"/>
+      <c r="D33" s="46"/>
+      <c r="E33" s="47"/>
+      <c r="F33" s="45"/>
+      <c r="G33" s="45"/>
+      <c r="H33" s="48"/>
+      <c r="I33" s="45"/>
+      <c r="J33" s="45"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A34" s="56"/>
-      <c r="B34" s="57"/>
-      <c r="C34" s="58"/>
-      <c r="D34" s="58"/>
-      <c r="E34" s="58"/>
-      <c r="F34" s="58"/>
-      <c r="G34" s="58"/>
-      <c r="H34" s="58"/>
-      <c r="I34" s="58"/>
-      <c r="J34" s="58"/>
+      <c r="A34" s="51"/>
+      <c r="B34" s="52"/>
+      <c r="C34" s="53"/>
+      <c r="D34" s="53"/>
+      <c r="E34" s="53"/>
+      <c r="F34" s="53"/>
+      <c r="G34" s="53"/>
+      <c r="H34" s="53"/>
+      <c r="I34" s="53"/>
+      <c r="J34" s="53"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A35" s="47"/>
-      <c r="B35" s="54"/>
-      <c r="C35" s="55"/>
-      <c r="D35" s="55"/>
-      <c r="E35" s="55"/>
-      <c r="F35" s="55"/>
-      <c r="G35" s="55"/>
-      <c r="H35" s="55"/>
-      <c r="I35" s="55"/>
-      <c r="J35" s="55"/>
+      <c r="A35" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35" s="49"/>
+      <c r="C35" s="50"/>
+      <c r="D35" s="50"/>
+      <c r="E35" s="50"/>
+      <c r="F35" s="50"/>
+      <c r="G35" s="50"/>
+      <c r="H35" s="50"/>
+      <c r="I35" s="50"/>
+      <c r="J35" s="50"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A36" s="47"/>
-      <c r="B36" s="54"/>
-      <c r="C36" s="55"/>
-      <c r="D36" s="55"/>
-      <c r="E36" s="55"/>
-      <c r="F36" s="55"/>
-      <c r="G36" s="55"/>
-      <c r="H36" s="55"/>
-      <c r="I36" s="55"/>
-      <c r="J36" s="55"/>
+      <c r="A36" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36" s="49"/>
+      <c r="C36" s="50"/>
+      <c r="D36" s="50"/>
+      <c r="E36" s="50"/>
+      <c r="F36" s="50"/>
+      <c r="G36" s="50"/>
+      <c r="H36" s="50"/>
+      <c r="I36" s="50"/>
+      <c r="J36" s="50"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A37" s="47"/>
-      <c r="B37" s="54"/>
-      <c r="C37" s="55"/>
-      <c r="D37" s="55"/>
-      <c r="E37" s="55"/>
-      <c r="F37" s="55"/>
-      <c r="G37" s="55"/>
-      <c r="H37" s="55"/>
-      <c r="I37" s="55"/>
-      <c r="J37" s="55"/>
+      <c r="A37" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37" s="49"/>
+      <c r="C37" s="50"/>
+      <c r="D37" s="50"/>
+      <c r="E37" s="50"/>
+      <c r="F37" s="50"/>
+      <c r="G37" s="50"/>
+      <c r="H37" s="50"/>
+      <c r="I37" s="50"/>
+      <c r="J37" s="50"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A38" s="47"/>
-      <c r="B38" s="54"/>
-      <c r="C38" s="55"/>
-      <c r="D38" s="55"/>
-      <c r="E38" s="55"/>
-      <c r="F38" s="55"/>
-      <c r="G38" s="55"/>
-      <c r="H38" s="55"/>
-      <c r="I38" s="55"/>
-      <c r="J38" s="55"/>
+      <c r="A38" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" s="49"/>
+      <c r="C38" s="50"/>
+      <c r="D38" s="50"/>
+      <c r="E38" s="50"/>
+      <c r="F38" s="50"/>
+      <c r="G38" s="50"/>
+      <c r="H38" s="50"/>
+      <c r="I38" s="50"/>
+      <c r="J38" s="50"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A39" s="47"/>
-      <c r="B39" s="54"/>
-      <c r="C39" s="55"/>
-      <c r="D39" s="55"/>
-      <c r="E39" s="55"/>
-      <c r="F39" s="55"/>
-      <c r="G39" s="55"/>
-      <c r="H39" s="55"/>
-      <c r="I39" s="55"/>
-      <c r="J39" s="55"/>
+      <c r="A39" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="B39" s="49"/>
+      <c r="C39" s="50"/>
+      <c r="D39" s="50"/>
+      <c r="E39" s="50"/>
+      <c r="F39" s="50"/>
+      <c r="G39" s="50"/>
+      <c r="H39" s="50"/>
+      <c r="I39" s="50"/>
+      <c r="J39" s="50"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A40" s="47"/>
-      <c r="B40" s="54"/>
-      <c r="C40" s="55"/>
-      <c r="D40" s="55"/>
-      <c r="E40" s="55"/>
-      <c r="F40" s="55"/>
-      <c r="G40" s="55"/>
-      <c r="H40" s="55"/>
-      <c r="I40" s="55"/>
-      <c r="J40" s="55"/>
+      <c r="A40" s="42"/>
+      <c r="B40" s="49"/>
+      <c r="C40" s="50"/>
+      <c r="D40" s="50"/>
+      <c r="E40" s="50"/>
+      <c r="F40" s="50"/>
+      <c r="G40" s="50"/>
+      <c r="H40" s="50"/>
+      <c r="I40" s="50"/>
+      <c r="J40" s="50"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A41" s="47"/>
-      <c r="B41" s="54"/>
-      <c r="C41" s="55"/>
-      <c r="D41" s="55"/>
-      <c r="E41" s="55"/>
-      <c r="F41" s="55"/>
-      <c r="G41" s="55"/>
-      <c r="H41" s="55"/>
-      <c r="I41" s="55"/>
-      <c r="J41" s="55"/>
+      <c r="A41" s="42"/>
+      <c r="B41" s="49"/>
+      <c r="C41" s="50"/>
+      <c r="D41" s="50"/>
+      <c r="E41" s="50"/>
+      <c r="F41" s="50"/>
+      <c r="G41" s="50"/>
+      <c r="H41" s="50"/>
+      <c r="I41" s="50"/>
+      <c r="J41" s="50"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A42" s="47"/>
-      <c r="B42" s="54"/>
-      <c r="C42" s="55"/>
-      <c r="D42" s="55"/>
-      <c r="E42" s="55"/>
-      <c r="F42" s="55"/>
-      <c r="G42" s="55"/>
-      <c r="H42" s="55"/>
-      <c r="I42" s="55"/>
-      <c r="J42" s="55"/>
+      <c r="A42" s="42"/>
+      <c r="B42" s="49"/>
+      <c r="C42" s="50"/>
+      <c r="D42" s="50"/>
+      <c r="E42" s="50"/>
+      <c r="F42" s="50"/>
+      <c r="G42" s="50"/>
+      <c r="H42" s="50"/>
+      <c r="I42" s="50"/>
+      <c r="J42" s="50"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A43" s="55"/>
-      <c r="B43" s="54"/>
-      <c r="C43" s="55"/>
-      <c r="D43" s="55"/>
-      <c r="E43" s="55"/>
-      <c r="F43" s="55"/>
-      <c r="G43" s="55"/>
-      <c r="H43" s="55"/>
-      <c r="I43" s="55"/>
-      <c r="J43" s="55"/>
+      <c r="A43" s="50"/>
+      <c r="B43" s="49"/>
+      <c r="C43" s="50"/>
+      <c r="D43" s="50"/>
+      <c r="E43" s="50"/>
+      <c r="F43" s="50"/>
+      <c r="G43" s="50"/>
+      <c r="H43" s="50"/>
+      <c r="I43" s="50"/>
+      <c r="J43" s="50"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B44" s="1"/>

</xml_diff>